<commit_message>
historial modificado vista apoderado
</commit_message>
<xml_diff>
--- a/database/seeds/Menu.xlsx
+++ b/database/seeds/Menu.xlsx
@@ -131,12 +131,6 @@
     <t>Historial Academico</t>
   </si>
   <si>
-    <t>historial_academico</t>
-  </si>
-  <si>
-    <t>HistorialAcademico</t>
-  </si>
-  <si>
     <t>Inscripciones</t>
   </si>
   <si>
@@ -303,6 +297,12 @@
   </si>
   <si>
     <t>AsignacionSeccionIndex</t>
+  </si>
+  <si>
+    <t>historial_pagos</t>
+  </si>
+  <si>
+    <t>HistorialPagos</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,13 +652,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D1">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -804,13 +804,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
         <v>80</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -922,13 +922,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
         <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -945,13 +945,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -971,10 +971,10 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -991,13 +991,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -1014,19 +1014,19 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1043,13 +1043,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1072,13 +1072,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
       </c>
       <c r="D19">
         <v>17</v>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
       </c>
       <c r="D20">
         <v>17</v>
@@ -1127,19 +1127,19 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1156,13 +1156,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -1185,13 +1185,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
         <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
       </c>
       <c r="D23">
         <v>21</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
         <v>61</v>
-      </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
       </c>
       <c r="D24">
         <v>21</v>
@@ -1243,13 +1243,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25">
         <v>21</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1295,13 +1295,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <v>26</v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28">
         <v>26</v>
@@ -1341,13 +1341,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30">
         <v>11</v>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
         <v>86</v>
-      </c>
-      <c r="B31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
       </c>
       <c r="D31">
         <v>1</v>

</xml_diff>